<commit_message>
Re-ran analysis for 5 layouts, considering cell chem
</commit_message>
<xml_diff>
--- a/failure_rates_computed.xlsx
+++ b/failure_rates_computed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alina/Documents/NREL/reliability/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8006CA-E63E-C644-9C89-8710C27FD515}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6431D33A-235A-5F46-8232-7F07FBC334F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35680" yWindow="-2260" windowWidth="26300" windowHeight="20260" xr2:uid="{7832D00E-6882-DC45-BF21-C249F4E48CEB}"/>
+    <workbookView xWindow="1420" yWindow="500" windowWidth="26300" windowHeight="16300" xr2:uid="{7832D00E-6882-DC45-BF21-C249F4E48CEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Calcs" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={2842E931-2AD5-A84E-803F-B07AEACE3D2A}</author>
+  </authors>
+  <commentList>
+    <comment ref="X6" authorId="0" shapeId="0" xr:uid="{2842E931-2AD5-A84E-803F-B07AEACE3D2A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    assuming balancing circuits operate for 20% of operating hours, or 10% of calendar hours</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="65">
   <si>
@@ -236,7 +254,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -272,6 +290,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -318,7 +342,9 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Alina Rossi-Conaway" id="{2F443F46-F71F-D14D-B7EC-25927055B793}" userId="S::rossi-conaway.a@northeastern.edu::73bf7853-892d-411e-a4f5-785152abc270" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -616,12 +642,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="X6" dT="2021-04-27T23:45:35.62" personId="{2F443F46-F71F-D14D-B7EC-25927055B793}" id="{2842E931-2AD5-A84E-803F-B07AEACE3D2A}">
+    <text>assuming balancing circuits operate for 20% of operating hours, or 10% of calendar hours</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682BB8FC-BBD4-C94B-8260-2E65D722EE22}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682BB8FC-BBD4-C94B-8260-2E65D722EE22}">
   <dimension ref="A1:AJ37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AD27" sqref="AD27"/>
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4053,6 +4087,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
modified spreadsheet slightly to include zener diode for passive balancing
</commit_message>
<xml_diff>
--- a/failure_rates_computed.xlsx
+++ b/failure_rates_computed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alina/Documents/NREL/reliability/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86792374-C33F-EE4C-9631-8772C491B60E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F6B6DA-2C68-9C42-8E09-FF713EA44A30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="500" windowWidth="26300" windowHeight="16300" xr2:uid="{7832D00E-6882-DC45-BF21-C249F4E48CEB}"/>
+    <workbookView xWindow="1420" yWindow="500" windowWidth="26300" windowHeight="16300" activeTab="1" xr2:uid="{7832D00E-6882-DC45-BF21-C249F4E48CEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Calcs" sheetId="1" r:id="rId1"/>
@@ -49,10 +49,10 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Columns A-T are computing component failure rates for power conversion systems—balancing system components use different operating conditions</t>
+    Columns A-R are computing component failure rates for power conversion systems—balancing system components use different operating conditions</t>
       </text>
     </comment>
-    <comment ref="T1" authorId="1" shapeId="0" xr:uid="{CBC231F0-E212-504F-9841-C93A0EA7C44B}">
+    <comment ref="R1" authorId="1" shapeId="0" xr:uid="{CBC231F0-E212-504F-9841-C93A0EA7C44B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -60,7 +60,7 @@
     All of these failure rates are for main converter components —balancing components have some different operating conditions</t>
       </text>
     </comment>
-    <comment ref="W1" authorId="2" shapeId="0" xr:uid="{51D6FA72-6CDC-6A4B-9058-02C6B69B3E70}">
+    <comment ref="U1" authorId="2" shapeId="0" xr:uid="{51D6FA72-6CDC-6A4B-9058-02C6B69B3E70}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -68,7 +68,7 @@
     Columns W-AJ compute failure rates for components in balancing circuits</t>
       </text>
     </comment>
-    <comment ref="X6" authorId="3" shapeId="0" xr:uid="{2842E931-2AD5-A84E-803F-B07AEACE3D2A}">
+    <comment ref="V6" authorId="3" shapeId="0" xr:uid="{2842E931-2AD5-A84E-803F-B07AEACE3D2A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -76,7 +76,7 @@
     assuming balancing circuits operate for 20% of operating hours, or 10% of calendar hours</t>
       </text>
     </comment>
-    <comment ref="W31" authorId="4" shapeId="0" xr:uid="{8F67F650-9BA8-CE4C-9E1A-3ACE019BCC5C}">
+    <comment ref="U31" authorId="4" shapeId="0" xr:uid="{8F67F650-9BA8-CE4C-9E1A-3ACE019BCC5C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -247,9 +247,6 @@
     <t>lambdaDiode_Schottky</t>
   </si>
   <si>
-    <t>lambdaDiode_Zener</t>
-  </si>
-  <si>
     <t>lambdaL</t>
   </si>
   <si>
@@ -271,9 +268,6 @@
     <t>lambdaMosfet_bal</t>
   </si>
   <si>
-    <t>lambdaDiode_bal</t>
-  </si>
-  <si>
     <t>lambdaC_bal</t>
   </si>
   <si>
@@ -284,13 +278,19 @@
   </si>
   <si>
     <t>lambdaR_bal</t>
+  </si>
+  <si>
+    <t>lambdaDiode_Abal</t>
+  </si>
+  <si>
+    <t>lambdaDiode_Pbal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -326,12 +326,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -681,18 +675,18 @@
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2021-04-29T14:55:13.37" personId="{2F443F46-F71F-D14D-B7EC-25927055B793}" id="{FF3B5A3F-F909-3343-AB16-D2ECEDD3A4E5}">
-    <text>Columns A-T are computing component failure rates for power conversion systems—balancing system components use different operating conditions</text>
+    <text>Columns A-R are computing component failure rates for power conversion systems—balancing system components use different operating conditions</text>
   </threadedComment>
-  <threadedComment ref="T1" dT="2021-04-29T14:53:10.27" personId="{2F443F46-F71F-D14D-B7EC-25927055B793}" id="{CBC231F0-E212-504F-9841-C93A0EA7C44B}">
+  <threadedComment ref="R1" dT="2021-04-29T14:53:10.27" personId="{2F443F46-F71F-D14D-B7EC-25927055B793}" id="{CBC231F0-E212-504F-9841-C93A0EA7C44B}">
     <text>All of these failure rates are for main converter components —balancing components have some different operating conditions</text>
   </threadedComment>
-  <threadedComment ref="W1" dT="2021-04-29T14:55:43.69" personId="{2F443F46-F71F-D14D-B7EC-25927055B793}" id="{51D6FA72-6CDC-6A4B-9058-02C6B69B3E70}">
+  <threadedComment ref="U1" dT="2021-04-29T14:55:43.69" personId="{2F443F46-F71F-D14D-B7EC-25927055B793}" id="{51D6FA72-6CDC-6A4B-9058-02C6B69B3E70}">
     <text>Columns W-AJ compute failure rates for components in balancing circuits</text>
   </threadedComment>
-  <threadedComment ref="X6" dT="2021-04-27T23:45:35.62" personId="{2F443F46-F71F-D14D-B7EC-25927055B793}" id="{2842E931-2AD5-A84E-803F-B07AEACE3D2A}">
+  <threadedComment ref="V6" dT="2021-04-27T23:45:35.62" personId="{2F443F46-F71F-D14D-B7EC-25927055B793}" id="{2842E931-2AD5-A84E-803F-B07AEACE3D2A}">
     <text>assuming balancing circuits operate for 20% of operating hours, or 10% of calendar hours</text>
   </threadedComment>
-  <threadedComment ref="W31" dT="2021-04-29T14:56:39.18" personId="{2F443F46-F71F-D14D-B7EC-25927055B793}" id="{8F67F650-9BA8-CE4C-9E1A-3ACE019BCC5C}">
+  <threadedComment ref="U31" dT="2021-04-29T14:56:39.18" personId="{2F443F46-F71F-D14D-B7EC-25927055B793}" id="{8F67F650-9BA8-CE4C-9E1A-3ACE019BCC5C}">
     <text>Neglecting “inductive” or “electrical overstress” failure rates for balancing components—I don’t expect them to be stressed that much and so I didn’t think it made sense for that failure rate to make such a large contribution to the overall failure rate</text>
   </threadedComment>
 </ThreadedComments>
@@ -702,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682BB8FC-BBD4-C94B-8260-2E65D722EE22}">
   <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U2" workbookViewId="0">
-      <selection activeCell="AD33" sqref="AD33"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AJ29" sqref="AJ29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,18 +706,18 @@
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10.83203125" style="3"/>
   </cols>
@@ -736,34 +730,34 @@
         <v>36</v>
       </c>
       <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" t="s">
         <v>41</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V1" t="s">
-        <v>47</v>
-      </c>
-      <c r="W1" t="s">
-        <v>42</v>
       </c>
       <c r="Y1" t="s">
         <v>36</v>
@@ -840,10 +834,10 @@
       <c r="R2">
         <v>40</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>0</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>40</v>
       </c>
       <c r="W2" t="s">
@@ -944,10 +938,10 @@
       <c r="R3">
         <v>14</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>1</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <v>14</v>
       </c>
       <c r="W3" t="s">
@@ -1048,10 +1042,10 @@
       <c r="R4">
         <v>0.5</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>2</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <v>0.5</v>
       </c>
       <c r="W4" t="s">
@@ -1152,10 +1146,10 @@
       <c r="R5">
         <v>2020</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>3</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>2020</v>
       </c>
       <c r="W5" t="s">
@@ -1256,11 +1250,11 @@
       <c r="R6">
         <v>0.5</v>
       </c>
-      <c r="S6" t="s">
+      <c r="U6" t="s">
         <v>4</v>
       </c>
-      <c r="T6">
-        <v>0.5</v>
+      <c r="V6">
+        <v>0.1</v>
       </c>
       <c r="W6" t="s">
         <v>4</v>
@@ -1365,24 +1359,25 @@
       <c r="R7">
         <v>365</v>
       </c>
-      <c r="S7" t="s">
+      <c r="U7" t="s">
         <v>5</v>
       </c>
-      <c r="T7">
-        <v>365</v>
+      <c r="V7">
+        <f>0.2*P7</f>
+        <v>73</v>
       </c>
       <c r="W7" t="s">
         <v>5</v>
       </c>
       <c r="X7">
-        <f>0.2*R7</f>
+        <f>Z7</f>
         <v>73</v>
       </c>
       <c r="Y7" t="s">
         <v>5</v>
       </c>
       <c r="Z7">
-        <f>0.2*T7</f>
+        <f>0.2*R7</f>
         <v>73</v>
       </c>
       <c r="AA7" t="s">
@@ -1476,10 +1471,10 @@
       <c r="R8">
         <v>0.5</v>
       </c>
-      <c r="S8" t="s">
+      <c r="U8" t="s">
         <v>6</v>
       </c>
-      <c r="T8">
+      <c r="V8">
         <v>0.5</v>
       </c>
       <c r="W8" t="s">
@@ -1542,7 +1537,7 @@
         <v>7</v>
       </c>
       <c r="F9">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="G9" t="s">
         <v>7</v>
@@ -1566,31 +1561,31 @@
         <v>7</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>0.39700000000000002</v>
       </c>
       <c r="O9" t="s">
         <v>7</v>
       </c>
       <c r="P9">
-        <v>0.39700000000000002</v>
+        <v>0.28100000000000003</v>
       </c>
       <c r="Q9" t="s">
         <v>7</v>
       </c>
       <c r="R9">
-        <v>0.28100000000000003</v>
-      </c>
-      <c r="S9" t="s">
+        <v>0</v>
+      </c>
+      <c r="U9" t="s">
         <v>7</v>
       </c>
-      <c r="T9">
-        <v>0</v>
+      <c r="V9">
+        <v>0.39700000000000002</v>
       </c>
       <c r="W9" t="s">
         <v>7</v>
       </c>
       <c r="X9">
-        <v>0.39700000000000002</v>
+        <v>0.15</v>
       </c>
       <c r="Y9" t="s">
         <v>7</v>
@@ -1649,7 +1644,7 @@
       </c>
       <c r="F10">
         <f>EXP(-F9*(F5-1993))</f>
-        <v>1.7422374639493515E-2</v>
+        <v>1</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -1677,35 +1672,35 @@
       </c>
       <c r="N10">
         <f>EXP(-N9*(N5-1993))</f>
-        <v>1</v>
+        <v>2.2120627803489172E-5</v>
       </c>
       <c r="O10" t="s">
         <v>8</v>
       </c>
       <c r="P10">
         <f>EXP(-P9*(P5-1993))</f>
-        <v>2.2120627803489172E-5</v>
+        <v>5.0699977406720709E-4</v>
       </c>
       <c r="Q10" t="s">
         <v>8</v>
       </c>
       <c r="R10">
         <f>EXP(-R9*(R5-1993))</f>
-        <v>5.0699977406720709E-4</v>
-      </c>
-      <c r="S10" t="s">
+        <v>1</v>
+      </c>
+      <c r="U10" t="s">
         <v>8</v>
       </c>
-      <c r="T10">
-        <f>EXP(-T9*(T5-1993))</f>
-        <v>1</v>
+      <c r="V10">
+        <f>EXP(-V9*(V5-1993))</f>
+        <v>2.2120627803489172E-5</v>
       </c>
       <c r="W10" t="s">
         <v>8</v>
       </c>
       <c r="X10">
         <f>EXP(-X9*(X5-1993))</f>
-        <v>2.2120627803489172E-5</v>
+        <v>1.7422374639493515E-2</v>
       </c>
       <c r="Y10" t="s">
         <v>8</v>
@@ -1767,55 +1762,55 @@
         <v>13</v>
       </c>
       <c r="F11">
-        <v>4.102E-4</v>
+        <v>7.9999999999999996E-7</v>
       </c>
       <c r="G11" t="s">
         <v>13</v>
       </c>
       <c r="H11">
-        <v>7.9999999999999996E-7</v>
+        <v>1.50145E-2</v>
       </c>
       <c r="I11" t="s">
         <v>13</v>
       </c>
       <c r="J11">
-        <v>1.50145E-2</v>
+        <v>1.214E-4</v>
       </c>
       <c r="K11" t="s">
         <v>13</v>
       </c>
       <c r="L11">
-        <v>1.214E-4</v>
+        <v>9.1299999999999997E-5</v>
       </c>
       <c r="M11" t="s">
         <v>13</v>
       </c>
       <c r="N11">
-        <v>9.1299999999999997E-5</v>
+        <v>1.049E-3</v>
       </c>
       <c r="O11" t="s">
         <v>13</v>
       </c>
       <c r="P11">
-        <v>1.049E-3</v>
+        <v>2.3499999999999999E-4</v>
       </c>
       <c r="Q11" t="s">
         <v>13</v>
       </c>
       <c r="R11">
-        <v>2.3499999999999999E-4</v>
-      </c>
-      <c r="S11" t="s">
+        <v>4.99E-5</v>
+      </c>
+      <c r="U11" t="s">
         <v>13</v>
       </c>
-      <c r="T11">
-        <v>4.99E-5</v>
+      <c r="V11">
+        <v>1.049E-3</v>
       </c>
       <c r="W11" t="s">
         <v>13</v>
       </c>
       <c r="X11">
-        <v>1.049E-3</v>
+        <v>4.102E-4</v>
       </c>
       <c r="Y11" t="s">
         <v>13</v>
@@ -1871,13 +1866,13 @@
         <v>14</v>
       </c>
       <c r="F12">
-        <v>0.23</v>
+        <v>0.4</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
       </c>
       <c r="H12">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="I12" t="s">
         <v>14</v>
@@ -1895,7 +1890,7 @@
         <v>14</v>
       </c>
       <c r="N12">
-        <v>0.38</v>
+        <v>0.23</v>
       </c>
       <c r="O12" t="s">
         <v>14</v>
@@ -1909,10 +1904,10 @@
       <c r="R12">
         <v>0.23</v>
       </c>
-      <c r="S12" t="s">
+      <c r="U12" t="s">
         <v>14</v>
       </c>
-      <c r="T12">
+      <c r="V12">
         <v>0.23</v>
       </c>
       <c r="W12" t="s">
@@ -1977,14 +1972,14 @@
       </c>
       <c r="F13">
         <f>F6/F12</f>
-        <v>2.1739130434782608</v>
+        <v>1.25</v>
       </c>
       <c r="G13" t="s">
         <v>15</v>
       </c>
       <c r="H13">
         <f>H6/H12</f>
-        <v>1.25</v>
+        <v>1.3157894736842106</v>
       </c>
       <c r="I13" t="s">
         <v>15</v>
@@ -2005,7 +2000,7 @@
       </c>
       <c r="N13">
         <f>N6/N12</f>
-        <v>1.3157894736842106</v>
+        <v>2.1739130434782608</v>
       </c>
       <c r="O13" t="s">
         <v>15</v>
@@ -2021,12 +2016,12 @@
         <f>R6/R12</f>
         <v>2.1739130434782608</v>
       </c>
-      <c r="S13" t="s">
+      <c r="U13" t="s">
         <v>15</v>
       </c>
-      <c r="T13">
-        <f>T6/T12</f>
-        <v>2.1739130434782608</v>
+      <c r="V13">
+        <f>V6/V12</f>
+        <v>0.43478260869565216</v>
       </c>
       <c r="W13" t="s">
         <v>15</v>
@@ -2095,13 +2090,13 @@
         <v>16</v>
       </c>
       <c r="F14">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
       <c r="G14" t="s">
         <v>16</v>
       </c>
       <c r="H14">
-        <v>0.47</v>
+        <v>0.24</v>
       </c>
       <c r="I14" t="s">
         <v>16</v>
@@ -2119,7 +2114,7 @@
         <v>16</v>
       </c>
       <c r="N14">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="O14" t="s">
         <v>16</v>
@@ -2133,10 +2128,10 @@
       <c r="R14">
         <v>0.2</v>
       </c>
-      <c r="S14" t="s">
+      <c r="U14" t="s">
         <v>16</v>
       </c>
-      <c r="T14">
+      <c r="V14">
         <v>0.2</v>
       </c>
       <c r="W14" t="s">
@@ -2200,13 +2195,13 @@
         <v>37</v>
       </c>
       <c r="F15">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G15" t="s">
         <v>37</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I15" t="s">
         <v>37</v>
@@ -2224,7 +2219,7 @@
         <v>37</v>
       </c>
       <c r="N15">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="O15" t="s">
         <v>37</v>
@@ -2236,13 +2231,13 @@
         <v>37</v>
       </c>
       <c r="R15">
+        <v>30</v>
+      </c>
+      <c r="U15" t="s">
+        <v>37</v>
+      </c>
+      <c r="V15">
         <v>60</v>
-      </c>
-      <c r="S15" t="s">
-        <v>37</v>
-      </c>
-      <c r="T15">
-        <v>30</v>
       </c>
       <c r="W15" t="s">
         <v>37</v>
@@ -2305,21 +2300,21 @@
         <v>17</v>
       </c>
       <c r="F16">
-        <f>EXP(-F14/0.00008617*(1/(F2+F15+273)-1/298))</f>
-        <v>4.7877761461441652</v>
+        <f>EXP((-F14/0.00008617)*(1/(F2+F15+273)-1/298))</f>
+        <v>2.4040314066929205</v>
       </c>
       <c r="G16" t="s">
         <v>17</v>
       </c>
       <c r="H16">
         <f>EXP((-H14/0.00008617)*(1/(H2+H15+273)-1/298))</f>
-        <v>2.4040314066929205</v>
+        <v>2.0614228462383903</v>
       </c>
       <c r="I16" t="s">
         <v>17</v>
       </c>
       <c r="J16">
-        <f>EXP((-J14/0.00008617)*(1/(J2+J15+273)-1/298))</f>
+        <f>EXP(-J14/0.00008617*(1/(J2+J15+273)-1/298))</f>
         <v>2.0614228462383903</v>
       </c>
       <c r="K16" t="s">
@@ -2334,7 +2329,7 @@
       </c>
       <c r="N16">
         <f>EXP(-N14/0.00008617*(1/(N2+N15+273)-1/298))</f>
-        <v>2.0614228462383903</v>
+        <v>4.7877761461441652</v>
       </c>
       <c r="O16" t="s">
         <v>17</v>
@@ -2348,14 +2343,14 @@
       </c>
       <c r="R16">
         <f>EXP(-R14/0.00008617*(1/(R2+R15+273)-1/298))</f>
+        <v>2.7782572522109406</v>
+      </c>
+      <c r="U16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V16">
+        <f>EXP(-V14/0.00008617*(1/(V2+V15+273)-1/298))</f>
         <v>4.7877761461441652</v>
-      </c>
-      <c r="S16" t="s">
-        <v>17</v>
-      </c>
-      <c r="T16">
-        <f>EXP(-T14/0.00008617*(1/(T2+T15+273)-1/298))</f>
-        <v>2.7782572522109406</v>
       </c>
       <c r="W16" t="s">
         <v>17</v>
@@ -2421,55 +2416,55 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="F17">
-        <v>0.28999999999999998</v>
+        <v>1.7999999999999999E-6</v>
       </c>
       <c r="G17" t="s">
         <v>21</v>
       </c>
       <c r="H17">
-        <v>1.7999999999999999E-6</v>
+        <v>8.5062999999999996E-3</v>
       </c>
       <c r="I17" t="s">
         <v>21</v>
       </c>
       <c r="J17">
-        <v>8.5062999999999996E-3</v>
+        <v>1.4990000000000001E-4</v>
       </c>
       <c r="K17" t="s">
         <v>21</v>
       </c>
       <c r="L17">
-        <v>1.4990000000000001E-4</v>
+        <v>4.1599999999999997E-4</v>
       </c>
       <c r="M17" t="s">
-        <v>21</v>
-      </c>
-      <c r="N17">
-        <v>4.1599999999999997E-4</v>
+        <v>38</v>
       </c>
       <c r="O17" t="s">
         <v>38</v>
       </c>
+      <c r="P17">
+        <v>0.5</v>
+      </c>
       <c r="Q17" t="s">
+        <v>45</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="U17" t="s">
         <v>38</v>
       </c>
-      <c r="R17">
-        <v>0.5</v>
-      </c>
-      <c r="S17" t="s">
-        <v>45</v>
-      </c>
-      <c r="T17" s="1">
-        <v>0.28999999999999998</v>
+      <c r="V17">
+        <v>0.5</v>
       </c>
       <c r="W17" t="s">
         <v>38</v>
       </c>
       <c r="X17">
-        <v>0.5</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="Y17" t="s">
         <v>38</v>
@@ -2524,17 +2519,16 @@
         <v>0.26696566317835924</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F18">
-        <f>F17^2.43/0.185</f>
-        <v>0.26696566317835924</v>
+        <v>0.6</v>
       </c>
       <c r="G18" t="s">
         <v>22</v>
       </c>
       <c r="H18">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="I18" t="s">
         <v>22</v>
@@ -2549,36 +2543,37 @@
         <v>0.62</v>
       </c>
       <c r="M18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="N18">
-        <v>0.62</v>
+        <v>1</v>
       </c>
       <c r="O18" t="s">
         <v>18</v>
       </c>
       <c r="P18">
+        <f>0.21*EXP(0.31*P17)</f>
+        <v>0.24520817183207624</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>46</v>
+      </c>
+      <c r="R18">
+        <f>(R17/0.29)^0.39</f>
         <v>1</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="U18" t="s">
         <v>18</v>
       </c>
-      <c r="R18">
-        <f>0.21*EXP(0.31*R17)</f>
-        <v>0.24520817183207624</v>
-      </c>
-      <c r="S18" t="s">
-        <v>46</v>
-      </c>
-      <c r="T18">
-        <f>(T17/0.29)^0.39</f>
+      <c r="V18">
         <v>1</v>
       </c>
       <c r="W18" t="s">
         <v>18</v>
       </c>
       <c r="X18">
-        <v>1</v>
+        <f>X17^2.43/0.185</f>
+        <v>0.26696566317835924</v>
       </c>
       <c r="Y18" t="s">
         <v>18</v>
@@ -2634,17 +2629,18 @@
         <v>6.0800000000000003E-4</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F19">
-        <v>9.8799999999999995E-4</v>
+        <f>(1-F6)/F18</f>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G19" t="s">
         <v>23</v>
       </c>
       <c r="H19">
         <f>(1-H6)/H18</f>
-        <v>0.83333333333333337</v>
+        <v>0.80645161290322587</v>
       </c>
       <c r="I19" t="s">
         <v>23</v>
@@ -2661,35 +2657,34 @@
         <v>0.80645161290322587</v>
       </c>
       <c r="M19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N19">
-        <f>(1-N6)/N18</f>
-        <v>0.80645161290322587</v>
+        <v>4.6739999999999998E-4</v>
       </c>
       <c r="O19" t="s">
         <v>21</v>
       </c>
       <c r="P19">
-        <v>4.6739999999999998E-4</v>
+        <v>1.6569999999999999E-4</v>
       </c>
       <c r="Q19" t="s">
         <v>21</v>
       </c>
       <c r="R19">
-        <v>1.6569999999999999E-4</v>
-      </c>
-      <c r="S19" t="s">
+        <v>4.5199999999999998E-4</v>
+      </c>
+      <c r="U19" t="s">
         <v>21</v>
       </c>
-      <c r="T19">
-        <v>4.5199999999999998E-4</v>
+      <c r="V19">
+        <v>4.6739999999999998E-4</v>
       </c>
       <c r="W19" t="s">
         <v>21</v>
       </c>
       <c r="X19">
-        <v>4.6739999999999998E-4</v>
+        <v>9.8799999999999995E-4</v>
       </c>
       <c r="Y19" t="s">
         <v>21</v>
@@ -2746,16 +2741,16 @@
         <v>0.77</v>
       </c>
       <c r="E20" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F20">
-        <v>0.77</v>
+        <v>0.08</v>
       </c>
       <c r="G20" t="s">
         <v>24</v>
       </c>
       <c r="H20">
-        <v>0.08</v>
+        <v>0.24</v>
       </c>
       <c r="I20" t="s">
         <v>24</v>
@@ -2770,10 +2765,10 @@
         <v>0.24</v>
       </c>
       <c r="M20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N20">
-        <v>0.24</v>
+        <v>0.77</v>
       </c>
       <c r="O20" t="s">
         <v>22</v>
@@ -2787,10 +2782,10 @@
       <c r="R20">
         <v>0.77</v>
       </c>
-      <c r="S20" t="s">
+      <c r="U20" t="s">
         <v>22</v>
       </c>
-      <c r="T20">
+      <c r="V20">
         <v>0.77</v>
       </c>
       <c r="W20" t="s">
@@ -2851,18 +2846,18 @@
         <v>0.64935064935064934</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F21">
-        <f>(1-F6)/F20</f>
-        <v>0.64935064935064934</v>
+        <f>EXP((-F20/0.00008617)*(1/(F3+273)-1/298))</f>
+        <v>0.88744687049516813</v>
       </c>
       <c r="G21" t="s">
         <v>25</v>
       </c>
       <c r="H21">
         <f>EXP((-H20/0.00008617)*(1/(H3+273)-1/298))</f>
-        <v>0.88744687049516813</v>
+        <v>0.69891938603078596</v>
       </c>
       <c r="I21" t="s">
         <v>25</v>
@@ -2879,11 +2874,11 @@
         <v>0.69891938603078596</v>
       </c>
       <c r="M21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N21">
-        <f>EXP((-N20/0.00008617)*(1/(N3+273)-1/298))</f>
-        <v>0.69891938603078596</v>
+        <f>(1-N6)/N20</f>
+        <v>0.64935064935064934</v>
       </c>
       <c r="O21" t="s">
         <v>23</v>
@@ -2899,12 +2894,12 @@
         <f>(1-R6)/R20</f>
         <v>0.64935064935064934</v>
       </c>
-      <c r="S21" t="s">
+      <c r="U21" t="s">
         <v>23</v>
       </c>
-      <c r="T21">
-        <f>(1-T6)/T20</f>
-        <v>0.64935064935064934</v>
+      <c r="V21">
+        <f>(1-V6)/V20</f>
+        <v>1.1688311688311688</v>
       </c>
       <c r="W21" t="s">
         <v>23</v>
@@ -2970,34 +2965,34 @@
         <v>0.4</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F22">
-        <v>0.3</v>
+        <v>2.9999999999999999E-7</v>
       </c>
       <c r="G22" t="s">
         <v>26</v>
       </c>
       <c r="H22">
-        <v>2.9999999999999999E-7</v>
+        <v>8.7950000000000007E-3</v>
       </c>
       <c r="I22" t="s">
         <v>26</v>
       </c>
       <c r="J22">
-        <v>8.7950000000000007E-3</v>
+        <v>5.1799999999999999E-5</v>
       </c>
       <c r="K22" t="s">
         <v>26</v>
       </c>
       <c r="L22">
-        <v>5.1799999999999999E-5</v>
+        <v>1.022E-4</v>
       </c>
       <c r="M22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N22">
-        <v>1.022E-4</v>
+        <v>0.3</v>
       </c>
       <c r="O22" t="s">
         <v>24</v>
@@ -3009,13 +3004,13 @@
         <v>24</v>
       </c>
       <c r="R22">
+        <v>0.2</v>
+      </c>
+      <c r="U22" t="s">
+        <v>24</v>
+      </c>
+      <c r="V22">
         <v>0.3</v>
-      </c>
-      <c r="S22" t="s">
-        <v>24</v>
-      </c>
-      <c r="T22">
-        <v>0.2</v>
       </c>
       <c r="W22" t="s">
         <v>24</v>
@@ -3076,17 +3071,16 @@
         <v>0.55044231312358938</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F23">
-        <f>EXP(-F22/0.00008617*(1/(F3+273)-1/298))</f>
-        <v>0.63904855683312856</v>
+        <v>413</v>
       </c>
       <c r="G23" t="s">
         <v>27</v>
       </c>
       <c r="H23">
-        <v>413</v>
+        <v>312</v>
       </c>
       <c r="I23" t="s">
         <v>27</v>
@@ -3101,10 +3095,11 @@
         <v>312</v>
       </c>
       <c r="M23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N23">
-        <v>312</v>
+        <f>EXP(-N22/0.00008617*(1/(N3+273)-1/298))</f>
+        <v>0.63904855683312856</v>
       </c>
       <c r="O23" t="s">
         <v>25</v>
@@ -3118,14 +3113,14 @@
       </c>
       <c r="R23">
         <f>EXP(-R22/0.00008617*(1/(R3+273)-1/298))</f>
+        <v>0.7419179962257213</v>
+      </c>
+      <c r="U23" t="s">
+        <v>25</v>
+      </c>
+      <c r="V23">
+        <f>EXP(-V22/0.00008617*(1/(V3+273)-1/298))</f>
         <v>0.63904855683312856</v>
-      </c>
-      <c r="S23" t="s">
-        <v>25</v>
-      </c>
-      <c r="T23">
-        <f>EXP(-T22/0.00008617*(1/(T3+273)-1/298))</f>
-        <v>0.7419179962257213</v>
       </c>
       <c r="W23" t="s">
         <v>25</v>
@@ -3187,17 +3182,18 @@
         <v>7.3999999999999999E-4</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F24">
-        <v>3.1999999999999999E-5</v>
+        <f>F7/F23</f>
+        <v>0.88377723970944311</v>
       </c>
       <c r="G24" t="s">
         <v>28</v>
       </c>
       <c r="H24">
         <f>H7/H23</f>
-        <v>0.88377723970944311</v>
+        <v>1.1698717948717949</v>
       </c>
       <c r="I24" t="s">
         <v>28</v>
@@ -3214,35 +3210,34 @@
         <v>1.1698717948717949</v>
       </c>
       <c r="M24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N24">
-        <f>N7/N23</f>
-        <v>1.1698717948717949</v>
+        <v>2.2499999999999999E-4</v>
       </c>
       <c r="O24" t="s">
         <v>26</v>
       </c>
       <c r="P24">
-        <v>2.2499999999999999E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="Q24" t="s">
         <v>26</v>
       </c>
       <c r="R24">
-        <v>1.6000000000000001E-4</v>
-      </c>
-      <c r="S24" t="s">
+        <v>1.4219999999999999E-4</v>
+      </c>
+      <c r="U24" t="s">
         <v>26</v>
       </c>
-      <c r="T24">
-        <v>1.4219999999999999E-4</v>
+      <c r="V24">
+        <v>2.2499999999999999E-4</v>
       </c>
       <c r="W24" t="s">
         <v>26</v>
       </c>
       <c r="X24">
-        <v>2.2499999999999999E-4</v>
+        <v>3.1999999999999999E-5</v>
       </c>
       <c r="Y24" t="s">
         <v>26</v>
@@ -3299,16 +3294,16 @@
         <v>736.84</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F25">
-        <v>736.82</v>
+        <v>8.94</v>
       </c>
       <c r="G25" t="s">
         <v>29</v>
       </c>
       <c r="H25">
-        <v>8.94</v>
+        <v>21.94</v>
       </c>
       <c r="I25" t="s">
         <v>29</v>
@@ -3323,10 +3318,10 @@
         <v>21.94</v>
       </c>
       <c r="M25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N25">
-        <v>21.94</v>
+        <v>754.38</v>
       </c>
       <c r="O25" t="s">
         <v>27</v>
@@ -3338,19 +3333,19 @@
         <v>27</v>
       </c>
       <c r="R25">
+        <v>1140.3499999999999</v>
+      </c>
+      <c r="U25" t="s">
+        <v>27</v>
+      </c>
+      <c r="V25">
         <v>754.38</v>
-      </c>
-      <c r="S25" t="s">
-        <v>27</v>
-      </c>
-      <c r="T25">
-        <v>1140.3499999999999</v>
       </c>
       <c r="W25" t="s">
         <v>27</v>
       </c>
       <c r="X25">
-        <v>754.38</v>
+        <v>736.82</v>
       </c>
       <c r="Y25" t="s">
         <v>27</v>
@@ -3405,18 +3400,18 @@
         <v>0.495358558167309</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F26">
-        <f>F7/F25</f>
-        <v>0.49537200401726333</v>
+        <f>((F2+F15-F3)/F25)^2</f>
+        <v>8.458077463978098</v>
       </c>
       <c r="G26" t="s">
         <v>30</v>
       </c>
       <c r="H26">
         <f>((H2+H15-H3)/H25)^2</f>
-        <v>8.458077463978098</v>
+        <v>2.6923514781757487</v>
       </c>
       <c r="I26" t="s">
         <v>30</v>
@@ -3433,11 +3428,11 @@
         <v>2.6923514781757487</v>
       </c>
       <c r="M26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N26">
-        <f>((N2+N15-N3)/N25)^2</f>
-        <v>2.6923514781757487</v>
+        <f>N7/N25</f>
+        <v>0.48384103502213738</v>
       </c>
       <c r="O26" t="s">
         <v>28</v>
@@ -3451,21 +3446,21 @@
       </c>
       <c r="R26">
         <f>R7/R25</f>
-        <v>0.48384103502213738</v>
-      </c>
-      <c r="S26" t="s">
+        <v>0.32007716929013025</v>
+      </c>
+      <c r="U26" t="s">
         <v>28</v>
       </c>
-      <c r="T26">
-        <f>T7/T25</f>
-        <v>0.32007716929013025</v>
+      <c r="V26">
+        <f>V7/V25</f>
+        <v>9.6768207004427481E-2</v>
       </c>
       <c r="W26" t="s">
         <v>28</v>
       </c>
       <c r="X26">
         <f>X7/X25</f>
-        <v>9.6768207004427481E-2</v>
+        <v>9.9074400803452672E-2</v>
       </c>
       <c r="Y26" t="s">
         <v>28</v>
@@ -3524,34 +3519,34 @@
         <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F27">
-        <v>80</v>
+        <v>1.9999999999999999E-7</v>
       </c>
       <c r="G27" t="s">
         <v>33</v>
       </c>
       <c r="H27">
-        <v>1.9999999999999999E-7</v>
+        <v>8.4979999999999995E-4</v>
       </c>
       <c r="I27" t="s">
         <v>33</v>
       </c>
       <c r="J27">
-        <v>8.4979999999999995E-4</v>
+        <v>3.8600000000000003E-5</v>
       </c>
       <c r="K27" t="s">
         <v>33</v>
       </c>
       <c r="L27">
-        <v>3.8600000000000003E-5</v>
+        <v>1.8199999999999999E-5</v>
       </c>
       <c r="M27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N27">
-        <v>1.8199999999999999E-5</v>
+        <v>80</v>
       </c>
       <c r="O27" t="s">
         <v>29</v>
@@ -3563,13 +3558,13 @@
         <v>29</v>
       </c>
       <c r="R27">
+        <v>86</v>
+      </c>
+      <c r="U27" t="s">
+        <v>29</v>
+      </c>
+      <c r="V27">
         <v>80</v>
-      </c>
-      <c r="S27" t="s">
-        <v>29</v>
-      </c>
-      <c r="T27">
-        <v>86</v>
       </c>
       <c r="W27" t="s">
         <v>29</v>
@@ -3630,39 +3625,39 @@
         <v>1.1556249999999999</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28">
-        <f>((F2+F15-F3)/F27)^2</f>
-        <v>1.1556249999999999</v>
+        <v>34</v>
+      </c>
+      <c r="F28" s="2">
+        <f>F10*(F11*F13*F16+F17*F19*F21+F22*F24*F26)+F27</f>
+        <v>6.1777186187446349E-6</v>
       </c>
       <c r="G28" t="s">
         <v>34</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="2">
         <f>H10*(H11*H13*H16+H17*H19*H21+H22*H24*H26)+H27</f>
-        <v>6.1777186187446349E-6</v>
+        <v>7.4071302394353208E-2</v>
       </c>
       <c r="I28" t="s">
         <v>34</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="2">
         <f>J10*(J11*J13*J16+J17*J19*J21+J22*J24*J26)+J27</f>
-        <v>7.4071302394353208E-2</v>
+        <v>6.1553028486934565E-4</v>
       </c>
       <c r="K28" t="s">
         <v>34</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="2">
         <f>L10*(L11*L13*L16+L17*L19*L21+L22*L24*L26)+L27</f>
-        <v>6.1553028486934565E-4</v>
+        <v>8.2221812146035945E-4</v>
       </c>
       <c r="M28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N28">
-        <f>N10*(N11*N13*N16+N17*N19*N21+N22*N24*N26)+N27</f>
-        <v>8.2221812146035945E-4</v>
+        <f>((N2+N15-N3)/N27)^2</f>
+        <v>1.1556249999999999</v>
       </c>
       <c r="O28" t="s">
         <v>30</v>
@@ -3676,14 +3671,14 @@
       </c>
       <c r="R28">
         <f>((R2+R15-R3)/R27)^2</f>
+        <v>0.42401297998918341</v>
+      </c>
+      <c r="U28" t="s">
+        <v>30</v>
+      </c>
+      <c r="V28">
+        <f>((V2+V15-V3)/V27)^2</f>
         <v>1.1556249999999999</v>
-      </c>
-      <c r="S28" t="s">
-        <v>30</v>
-      </c>
-      <c r="T28">
-        <f>((T2+T15-T3)/T27)^2</f>
-        <v>0.42401297998918341</v>
       </c>
       <c r="W28" t="s">
         <v>30</v>
@@ -3747,19 +3742,11 @@
       <c r="D29">
         <v>2.1000000000000001E-4</v>
       </c>
-      <c r="E29" t="s">
+      <c r="M29" t="s">
         <v>31</v>
       </c>
-      <c r="F29">
-        <v>2.1000000000000001E-4</v>
-      </c>
-      <c r="H29">
-        <f>H28-H27</f>
-        <v>5.9777186187446351E-6</v>
-      </c>
-      <c r="J29">
-        <f>J28-J27</f>
-        <v>7.3221502394353211E-2</v>
+      <c r="N29">
+        <v>1.5E-3</v>
       </c>
       <c r="O29" t="s">
         <v>31</v>
@@ -3771,19 +3758,19 @@
         <v>31</v>
       </c>
       <c r="R29">
+        <v>8.8999999999999995E-4</v>
+      </c>
+      <c r="U29" t="s">
+        <v>31</v>
+      </c>
+      <c r="V29">
         <v>1.5E-3</v>
-      </c>
-      <c r="S29" t="s">
-        <v>31</v>
-      </c>
-      <c r="T29">
-        <v>8.8999999999999995E-4</v>
       </c>
       <c r="W29" t="s">
         <v>31</v>
       </c>
       <c r="X29">
-        <v>1.5E-3</v>
+        <v>2.1000000000000001E-4</v>
       </c>
       <c r="Y29" t="s">
         <v>31</v>
@@ -3797,7 +3784,7 @@
       <c r="AB29">
         <v>1140.3499999999999</v>
       </c>
-      <c r="AD29">
+      <c r="AD29" s="2">
         <f>AD28-AD27</f>
         <v>3.3254162129373304E-6</v>
       </c>
@@ -3812,7 +3799,7 @@
       <c r="AH29">
         <v>8.8999999999999995E-4</v>
       </c>
-      <c r="AJ29">
+      <c r="AJ29" s="2">
         <f>AJ28-AJ27</f>
         <v>5.3596551408408087E-4</v>
       </c>
@@ -3832,11 +3819,11 @@
         <f>((D2+D15-D3)/44)^2.26</f>
         <v>4.5474030731965112</v>
       </c>
-      <c r="E30" t="s">
+      <c r="M30" t="s">
         <v>32</v>
       </c>
-      <c r="F30">
-        <f>((F2+F15-F3)/44)^2.26</f>
+      <c r="N30">
+        <f>((N2+N15-N3)/44)^2.26</f>
         <v>4.5474030731965112</v>
       </c>
       <c r="O30" t="s">
@@ -3851,14 +3838,14 @@
       </c>
       <c r="R30">
         <f>((R2+R15-R3)/44)^2.26</f>
+        <v>1.7246536511918495</v>
+      </c>
+      <c r="U30" t="s">
+        <v>32</v>
+      </c>
+      <c r="V30">
+        <f>((V2+V15-V3)/44)^2.26</f>
         <v>4.5474030731965112</v>
-      </c>
-      <c r="S30" t="s">
-        <v>32</v>
-      </c>
-      <c r="T30">
-        <f>((T2+T15-T3)/44)^2.26</f>
-        <v>1.7246536511918495</v>
       </c>
       <c r="W30" t="s">
         <v>32</v>
@@ -3902,35 +3889,35 @@
       <c r="D31">
         <v>3.16E-3</v>
       </c>
-      <c r="E31" t="s">
+      <c r="M31" t="s">
         <v>33</v>
       </c>
-      <c r="F31">
-        <v>2.2599999999999999E-3</v>
+      <c r="N31">
+        <v>4.5409999999999999E-2</v>
       </c>
       <c r="O31" t="s">
         <v>33</v>
       </c>
       <c r="P31">
-        <v>4.5409999999999999E-2</v>
+        <v>8.8990000000000007E-3</v>
       </c>
       <c r="Q31" t="s">
         <v>33</v>
       </c>
       <c r="R31">
-        <v>8.8990000000000007E-3</v>
-      </c>
-      <c r="S31" t="s">
+        <v>5.2590000000000004E-4</v>
+      </c>
+      <c r="U31" t="s">
         <v>33</v>
       </c>
-      <c r="T31">
-        <v>5.2590000000000004E-4</v>
+      <c r="V31">
+        <v>4.5409999999999999E-2</v>
       </c>
       <c r="W31" t="s">
         <v>33</v>
       </c>
       <c r="X31">
-        <v>4.5409999999999999E-2</v>
+        <v>2.2599999999999999E-3</v>
       </c>
       <c r="Y31" t="s">
         <v>33</v>
@@ -3962,44 +3949,44 @@
       <c r="C32" t="s">
         <v>34</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <f>D10*(D11*D13*D16*D18+D19*D21*D23+D24*D26*D28)+D29*D30+D31</f>
         <v>4.1181735002985206E-3</v>
       </c>
-      <c r="E32" t="s">
+      <c r="M32" t="s">
         <v>34</v>
       </c>
-      <c r="F32">
-        <f>F10*(F11*F13*F16*F18+F19*F21*F23+F24*F26*F28)+F29*F30+F31</f>
-        <v>3.2422747005345261E-3</v>
+      <c r="N32" s="2">
+        <f>N10*(N11*N13*N16*N18+N19*N21*N23+N24*N26*N28)+N29*N30+N31</f>
+        <v>5.2231353200809905E-2</v>
       </c>
       <c r="O32" t="s">
         <v>34</v>
       </c>
-      <c r="P32">
+      <c r="P32" s="2">
         <f>P10*(P11*P13*P16*P18+P19*P21*P23+P24*P26*P28)+P29*P30+P31</f>
-        <v>5.2231353200809905E-2</v>
+        <v>1.5720488907501228E-2</v>
       </c>
       <c r="Q32" t="s">
         <v>34</v>
       </c>
-      <c r="R32">
+      <c r="R32" s="2">
         <f>R10*(R11*R13*R16*R18+R19*R21*R23+R24*R26*R28)+R29*R30+R31</f>
-        <v>1.5720488907501228E-2</v>
-      </c>
-      <c r="S32" t="s">
+        <v>2.599278953606861E-3</v>
+      </c>
+      <c r="U32" t="s">
         <v>34</v>
       </c>
-      <c r="T32">
-        <f>T10*(T11*T13*T16*T18+T19*T21*T23+T24*T26*T28)+T29*T30+T31</f>
-        <v>2.599278953606861E-3</v>
+      <c r="V32">
+        <f>V10*(V11*V13*V16*V18+V19*V21*V23+V24*V26*V28)+V29*V30+V31</f>
+        <v>5.2231161192661663E-2</v>
       </c>
       <c r="W32" t="s">
         <v>34</v>
       </c>
       <c r="X32">
         <f>X10*(X11*X13*X16*X18+X19*X21*X23+X24*X26*X28)+X29*X30+X31</f>
-        <v>5.2231161192661663E-2</v>
+        <v>3.2318473716761629E-3</v>
       </c>
       <c r="Y32" t="s">
         <v>34</v>
@@ -4030,31 +4017,16 @@
       <c r="B33">
         <v>9.5E-4</v>
       </c>
-      <c r="D33">
-        <f>D32-D31</f>
-        <v>9.5817350029852059E-4</v>
-      </c>
-      <c r="F33">
-        <f>F32-F31</f>
-        <v>9.8227470053452622E-4</v>
-      </c>
-      <c r="P33" s="2">
-        <f>P32-P31</f>
-        <v>6.8213532008099056E-3</v>
-      </c>
-      <c r="R33">
-        <f>R32-R31</f>
-        <v>6.8214889075012275E-3</v>
-      </c>
-      <c r="T33">
-        <f>T32-T31</f>
-        <v>2.0733789536068609E-3</v>
-      </c>
-      <c r="X33">
+      <c r="N33" s="2"/>
+      <c r="V33" s="2">
+        <f>V32-V31</f>
+        <v>6.8211611926616636E-3</v>
+      </c>
+      <c r="X33" s="2">
         <f>X32-X31</f>
-        <v>6.8211611926616636E-3</v>
-      </c>
-      <c r="Z33">
+        <v>9.7184737167616301E-4</v>
+      </c>
+      <c r="Z33" s="2">
         <f>Z32-Z31</f>
         <v>9.564423874594088E-4</v>
       </c>
@@ -4064,7 +4036,7 @@
       <c r="AB33">
         <v>9.5E-4</v>
       </c>
-      <c r="AH33">
+      <c r="AH33" s="2">
         <f>AH32-AH31</f>
         <v>1.9910415896364896E-3</v>
       </c>
@@ -4077,14 +4049,6 @@
         <f>((B2-B3)/44)^2.26</f>
         <v>0.30453465258122364</v>
       </c>
-      <c r="D34">
-        <f>D32/10^6</f>
-        <v>4.1181735002985203E-9</v>
-      </c>
-      <c r="P34">
-        <f>P32/10^6</f>
-        <v>5.2231353200809902E-8</v>
-      </c>
       <c r="AA34" t="s">
         <v>32</v>
       </c>
@@ -4111,7 +4075,7 @@
       <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <f>B10*B14*(B15*B17*B19*B22+B23*B25*B27+B28*B30*B32)+B33*B34+B35</f>
         <v>1.3785264806911732E-3</v>
       </c>
@@ -4124,11 +4088,7 @@
       </c>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B37">
-        <f>B36-B35</f>
-        <v>1.1195264806911731E-3</v>
-      </c>
-      <c r="AB37">
+      <c r="AB37" s="2">
         <f>AB36-AB35</f>
         <v>6.2050844218532381E-4</v>
       </c>
@@ -4143,7 +4103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B856A50-D67C-A241-8B81-145174D9959D}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -4176,35 +4136,35 @@
         <v>52</v>
       </c>
       <c r="B3">
-        <f>Calcs!F32</f>
-        <v>3.2422747005345261E-3</v>
+        <f>Calcs!F28</f>
+        <v>6.1777186187446349E-6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4">
-        <f>Calcs!H28</f>
-        <v>6.1777186187446349E-6</v>
+        <f>3*Calcs!J28</f>
+        <v>1.8465908546080371E-3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5">
-        <f>3*Calcs!L28</f>
-        <v>1.8465908546080371E-3</v>
+        <f>Calcs!L28</f>
+        <v>8.2221812146035945E-4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B6">
-        <f>Calcs!N28</f>
-        <v>8.2221812146035945E-4</v>
+        <f>Calcs!N32</f>
+        <v>5.2231353200809905E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -4213,7 +4173,7 @@
       </c>
       <c r="B7">
         <f>Calcs!P32</f>
-        <v>5.2231353200809905E-2</v>
+        <v>1.5720488907501228E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -4222,7 +4182,7 @@
       </c>
       <c r="B8">
         <f>Calcs!R32</f>
-        <v>1.5720488907501228E-2</v>
+        <v>2.599278953606861E-3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -4230,22 +4190,22 @@
         <v>58</v>
       </c>
       <c r="B9">
-        <f>Calcs!T32</f>
-        <v>2.599278953606861E-3</v>
+        <f>Calcs!V33</f>
+        <v>6.8211611926616636E-3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B10">
         <f>Calcs!X33</f>
-        <v>6.8211611926616636E-3</v>
+        <v>9.7184737167616301E-4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B11">
         <f>Calcs!Z33</f>
@@ -4254,7 +4214,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12">
         <f>Calcs!AB37</f>
@@ -4263,7 +4223,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13">
         <f>Calcs!AD29</f>
@@ -4272,7 +4232,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B14">
         <f>Calcs!AH33</f>
@@ -4281,7 +4241,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B15">
         <f>Calcs!AJ29</f>

</xml_diff>